<commit_message>
pipeline nearly done, just sample performance log has issues
</commit_message>
<xml_diff>
--- a/data/Leetcode_question_log.xlsx
+++ b/data/Leetcode_question_log.xlsx
@@ -6486,8 +6486,12 @@
       </c>
       <c r="I175" t="inlineStr"/>
       <c r="J175" t="inlineStr"/>
-      <c r="K175" t="inlineStr"/>
-      <c r="L175" t="inlineStr"/>
+      <c r="K175" t="n">
+        <v>1</v>
+      </c>
+      <c r="L175" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="176">
       <c r="A176" t="n">
@@ -9422,8 +9426,12 @@
       </c>
       <c r="I260" t="inlineStr"/>
       <c r="J260" t="inlineStr"/>
-      <c r="K260" t="inlineStr"/>
-      <c r="L260" t="inlineStr"/>
+      <c r="K260" t="n">
+        <v>1</v>
+      </c>
+      <c r="L260" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="261">
       <c r="A261" t="n">
@@ -11166,8 +11174,12 @@
       </c>
       <c r="I311" t="inlineStr"/>
       <c r="J311" t="inlineStr"/>
-      <c r="K311" t="inlineStr"/>
-      <c r="L311" t="inlineStr"/>
+      <c r="K311" t="n">
+        <v>1</v>
+      </c>
+      <c r="L311" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="312">
       <c r="A312" t="n">
@@ -17240,8 +17252,12 @@
       </c>
       <c r="I488" t="inlineStr"/>
       <c r="J488" t="inlineStr"/>
-      <c r="K488" t="inlineStr"/>
-      <c r="L488" t="inlineStr"/>
+      <c r="K488" t="n">
+        <v>1</v>
+      </c>
+      <c r="L488" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="489">
       <c r="A489" t="n">
@@ -22648,8 +22664,12 @@
       </c>
       <c r="I645" t="inlineStr"/>
       <c r="J645" t="inlineStr"/>
-      <c r="K645" t="inlineStr"/>
-      <c r="L645" t="inlineStr"/>
+      <c r="K645" t="n">
+        <v>1</v>
+      </c>
+      <c r="L645" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="646">
       <c r="A646" t="n">
@@ -25896,8 +25916,12 @@
       </c>
       <c r="I739" t="inlineStr"/>
       <c r="J739" t="inlineStr"/>
-      <c r="K739" t="inlineStr"/>
-      <c r="L739" t="inlineStr"/>
+      <c r="K739" t="n">
+        <v>1</v>
+      </c>
+      <c r="L739" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="740">
       <c r="A740" t="n">
@@ -26104,8 +26128,12 @@
       </c>
       <c r="I745" t="inlineStr"/>
       <c r="J745" t="inlineStr"/>
-      <c r="K745" t="inlineStr"/>
-      <c r="L745" t="inlineStr"/>
+      <c r="K745" t="n">
+        <v>1</v>
+      </c>
+      <c r="L745" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="746">
       <c r="A746" t="n">
@@ -26732,7 +26760,9 @@
       </c>
       <c r="I763" t="inlineStr"/>
       <c r="J763" t="inlineStr"/>
-      <c r="K763" t="inlineStr"/>
+      <c r="K763" t="n">
+        <v>1</v>
+      </c>
       <c r="L763" t="inlineStr"/>
     </row>
     <row r="764">
@@ -28962,7 +28992,9 @@
       </c>
       <c r="I828" t="inlineStr"/>
       <c r="J828" t="inlineStr"/>
-      <c r="K828" t="inlineStr"/>
+      <c r="K828" t="n">
+        <v>1</v>
+      </c>
       <c r="L828" t="inlineStr"/>
     </row>
     <row r="829">
@@ -42830,8 +42862,12 @@
       </c>
       <c r="I1232" t="inlineStr"/>
       <c r="J1232" t="inlineStr"/>
-      <c r="K1232" t="inlineStr"/>
-      <c r="L1232" t="inlineStr"/>
+      <c r="K1232" t="n">
+        <v>1</v>
+      </c>
+      <c r="L1232" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="1233">
       <c r="A1233" t="n">

</xml_diff>